<commit_message>
Working on next button
</commit_message>
<xml_diff>
--- a/cobourg_rental_properties.xlsx
+++ b/cobourg_rental_properties.xlsx
@@ -458,215 +458,215 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>417 TREVOR STREET, Cobourg, Ontario</t>
+          <t>232 NICKERSON DRIVE, Cobourg, Ontario</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$2,900/Monthly</t>
+          <t>$2,700/Monthly</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>3 + 1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>B - 92 ORANGE STREET, Cobourg, Ontario</t>
+          <t>LOT 114 - 1081 DENTON DRIVE, Cobourg, Ontario</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>$1,900/Monthly</t>
+          <t>$3,500/Monthly</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4 + 1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>502 - 79 KING STREET, Cobourg, Ontario</t>
+          <t>404 - 325 UNIVERSITY AVENUE W, Cobourg, Ontario</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>$2,650/Monthly</t>
+          <t>$2,025/Monthly</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>475 DREWERY ROAD, Cobourg, Ontario</t>
+          <t>1016 TRAILSVIEW AVENUE, Cobourg, Ontario</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>$3,200/Monthly</t>
+          <t>$3,499/Monthly</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>27 - 160 DENSMORE ROAD, Cobourg, Ontario</t>
+          <t>UNIT 1 - 74 KING STREET W, Cobourg, Ontario</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>$2,890/Monthly</t>
+          <t>$1,600/Monthly</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1066 DENTON DRIVE, Cobourg, Ontario</t>
+          <t>319 - 325 UNIVERSITY AVENUE W, Cobourg, Ontario</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$3,400/Monthly</t>
+          <t>$2,050/Monthly</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>26 SPENCER STREET, Cobourg, Ontario</t>
+          <t>1004 TRAILSVIEW AVENUE, Cobourg, Ontario</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>$1,850/Monthly</t>
+          <t>$3,500/Monthly</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>217 - 325 UNIVERSITY AVENUE W, Cobourg, Ontario</t>
+          <t>417 TREVOR STREET, Cobourg, Ontario</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>$2,050/Monthly</t>
+          <t>$2,900/Monthly</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1 + 1</t>
+          <t>3 + 1</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>540 TREVOR STREET, Cobourg, Ontario</t>
+          <t>502 - 79 KING STREET, Cobourg, Ontario</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>$3,300/Monthly</t>
+          <t>$2,650/Monthly</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>498 HORNBECK STREET, Cobourg, Ontario</t>
+          <t>475 DREWERY ROAD, Cobourg, Ontario</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>$3,300/Monthly</t>
+          <t>$3,200/Monthly</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -678,17 +678,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>488 TREVOR STREET, Cobourg, Ontario</t>
+          <t>27 - 160 DENSMORE ROAD, Cobourg, Ontario</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>$3,100/Monthly</t>
+          <t>$2,890/Monthly</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -700,12 +700,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>883 CARLISLE STREET, Cobourg, Ontario</t>
+          <t>1066 DENTON DRIVE, Cobourg, Ontario</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>$4,500/Monthly</t>
+          <t>$3,400/Monthly</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -715,7 +715,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>

</xml_diff>